<commit_message>
BR : Rename main1.py to main.py
</commit_message>
<xml_diff>
--- a/Output/HLB Mann Judd Brisbane, Queensland (HLB Australia).xlsx
+++ b/Output/HLB Mann Judd Brisbane, Queensland (HLB Australia).xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Work Referred inc amavat 2021" sheetId="1" r:id="rId1"/>
+    <sheet name="Work Received inc amavat 2021" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -491,225 +491,240 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:13">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:14">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
-      <c r="A2" t="s">
+    <row r="2" spans="1:14">
+      <c r="A2" s="1">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>16</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>18</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>22</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>1652.710446</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>165.2710446</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>26</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>29</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>32</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>34</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
-      <c r="A3" t="s">
+    <row r="3" spans="1:14">
+      <c r="A3" s="1">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>17</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>19</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>23</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>3305.420892000001</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>330.5420892000001</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>26</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>27</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>29</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>33</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>35</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
-      <c r="A4" t="s">
+    <row r="4" spans="1:14">
+      <c r="A4" s="1">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>14</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>16</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>20</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>24</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>578.4486561000001</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>57.84486561000001</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>26</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>28</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>30</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>33</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>36</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
-      <c r="A5" t="s">
+    <row r="5" spans="1:14">
+      <c r="A5" s="1">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>16</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>21</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>25</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>1680.2556201</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>168.02556201</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>26</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>28</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>31</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>33</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>34</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
-      <c r="B6" t="s">
+    <row r="6" spans="1:14">
+      <c r="A6" s="1">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
         <v>15</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>7216.835614200001</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>721.6835614200002</v>
       </c>
     </row>

</xml_diff>